<commit_message>
ajout de fichier de conversion Excel en xml
</commit_message>
<xml_diff>
--- a/resources/AP1/Modules.xlsx
+++ b/resources/AP1/Modules.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\xml_projekt\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\GestionScolarite-XML\resources\AP1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{464DD101-243D-49F5-BD10-6D8AE12ACFE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B30EAF57-9662-43DC-8C7D-DCB2385990AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9915" yWindow="315" windowWidth="10575" windowHeight="10530" xr2:uid="{4B6EDB86-5034-44F2-BBEE-2F607F14F8DA}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{4B6EDB86-5034-44F2-BBEE-2F607F14F8DA}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -168,31 +166,31 @@
     <t>CodeModule</t>
   </si>
   <si>
-    <t>AP21</t>
-  </si>
-  <si>
-    <t>AP22</t>
-  </si>
-  <si>
-    <t>AP23</t>
-  </si>
-  <si>
-    <t>AP24</t>
-  </si>
-  <si>
-    <t>AP25</t>
-  </si>
-  <si>
-    <t>AP26</t>
-  </si>
-  <si>
-    <t>AP27</t>
-  </si>
-  <si>
-    <t>AP28</t>
-  </si>
-  <si>
-    <t>AP29</t>
+    <t>AP11</t>
+  </si>
+  <si>
+    <t>AP12</t>
+  </si>
+  <si>
+    <t>AP13</t>
+  </si>
+  <si>
+    <t>AP14</t>
+  </si>
+  <si>
+    <t>AP15</t>
+  </si>
+  <si>
+    <t>AP16</t>
+  </si>
+  <si>
+    <t>AP17</t>
+  </si>
+  <si>
+    <t>AP18</t>
+  </si>
+  <si>
+    <t>AP19</t>
   </si>
 </sst>
 </file>
@@ -552,218 +550,218 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD852E43-8D03-4FFF-B12B-9429ED06A3DA}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" customWidth="1"/>
+    <col min="1" max="1" width="16.7265625" customWidth="1"/>
+    <col min="2" max="2" width="20.81640625" customWidth="1"/>
+    <col min="3" max="3" width="19.26953125" customWidth="1"/>
+    <col min="4" max="4" width="21.453125" customWidth="1"/>
+    <col min="5" max="5" width="16.1796875" customWidth="1"/>
+    <col min="6" max="6" width="13.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>13</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>15</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>16</v>
       </c>
-      <c r="F3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" t="s">
         <v>17</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>18</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>19</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>15</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>20</v>
       </c>
-      <c r="F4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" t="s">
         <v>0</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>21</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>22</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>10</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>23</v>
       </c>
-      <c r="F5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" t="s">
         <v>24</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>25</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>26</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>10</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>27</v>
       </c>
-      <c r="F6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" t="s">
         <v>28</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>29</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>30</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>10</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>31</v>
       </c>
-      <c r="F7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" t="s">
         <v>1</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>32</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>33</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>10</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>34</v>
       </c>
-      <c r="F8" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" t="s">
         <v>35</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>36</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>37</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>10</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>38</v>
       </c>
-      <c r="F9" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" t="s">
         <v>39</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>40</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>41</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>10</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>42</v>
-      </c>
-      <c r="F10" t="s">
-        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>